<commit_message>
Lista sección 12 :)
</commit_message>
<xml_diff>
--- a/Documentación/Tablas/12-1 Descripción de los módulos - BOMs.xlsx
+++ b/Documentación/Tablas/12-1 Descripción de los módulos - BOMs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\Wet-DryPenguins\Documentación\Tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFF71F-DA9B-4555-BDC3-56CA019AD9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6750762-2475-4086-A806-2011DA3C27C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM Base" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM Logger" sheetId="2" r:id="rId1"/>
+    <sheet name="BOM Base" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Componente</t>
   </si>
@@ -94,6 +95,69 @@
   </si>
   <si>
     <t>Código</t>
+  </si>
+  <si>
+    <t>MSP430FR2476TRHBR</t>
+  </si>
+  <si>
+    <t>Diodo Schottky</t>
+  </si>
+  <si>
+    <t>CDBQR70</t>
+  </si>
+  <si>
+    <t>Diodo Rectificador</t>
+  </si>
+  <si>
+    <t>1N4148WL2-TP</t>
+  </si>
+  <si>
+    <t>LED Verde</t>
+  </si>
+  <si>
+    <t>LTST-C171GKT</t>
+  </si>
+  <si>
+    <t>Capacitor 100n</t>
+  </si>
+  <si>
+    <t>CL05B104KP5VPNC</t>
+  </si>
+  <si>
+    <t>Capacitor 4.7n</t>
+  </si>
+  <si>
+    <t>C0402C472K5RECAUTO</t>
+  </si>
+  <si>
+    <t>RES100</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100RL</t>
+  </si>
+  <si>
+    <t>RES47K</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ473X</t>
+  </si>
+  <si>
+    <t>RES2K2</t>
+  </si>
+  <si>
+    <t>RC0402FR-072K2L</t>
+  </si>
+  <si>
+    <t>Pines</t>
+  </si>
+  <si>
+    <t>6136-0-00-15-00-00-03-0</t>
+  </si>
+  <si>
+    <t>Pilas</t>
+  </si>
+  <si>
+    <t>SR626</t>
   </si>
 </sst>
 </file>
@@ -162,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +240,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,13 +543,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CDF7D6-F58D-4999-ABBB-A8E2775DA09B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6">
+        <f>4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>